<commit_message>
adding power query file
</commit_message>
<xml_diff>
--- a/movies_db_index_match.xlsx
+++ b/movies_db_index_match.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teja5\Desktop\pandu\excel_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6787FF85-995F-42A9-B1D0-A4803685FE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F923C88-6AFB-4F4B-AB03-7135DAAEE040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="movies" sheetId="1" r:id="rId1"/>
-    <sheet name="financials" sheetId="2" r:id="rId2"/>
-    <sheet name="actors" sheetId="3" r:id="rId3"/>
-    <sheet name="movie_actor" sheetId="4" r:id="rId4"/>
-    <sheet name="languages" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="financials" sheetId="2" r:id="rId3"/>
+    <sheet name="actors" sheetId="3" r:id="rId4"/>
+    <sheet name="movie_actor" sheetId="4" r:id="rId5"/>
+    <sheet name="languages" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="185">
   <si>
     <t>movie_id</t>
   </si>
@@ -512,13 +513,91 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>Budget (Mln)</t>
+  </si>
+  <si>
+    <t>Revenue (Mln)</t>
+  </si>
+  <si>
+    <t>Budget INR</t>
+  </si>
+  <si>
+    <t>Revenue INR</t>
+  </si>
+  <si>
+    <t>Budget USD</t>
+  </si>
+  <si>
+    <t>Revenue USD</t>
+  </si>
+  <si>
+    <t>Total No.of MOVIES</t>
+  </si>
+  <si>
+    <t>BOLLYWOOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Bollywood Budget INR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Bollywood Revenue INR </t>
+  </si>
+  <si>
+    <t>Avg Bollywood Revenue INR</t>
+  </si>
+  <si>
+    <t>% of revenue from INR</t>
+  </si>
+  <si>
+    <t>Key Matric</t>
+  </si>
+  <si>
+    <t>Marvel Consolidated  P&amp; L</t>
+  </si>
+  <si>
+    <t>Profit /Loss</t>
+  </si>
+  <si>
+    <t>Profit /Loss %</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market share % </t>
+  </si>
+  <si>
+    <t>Actual -Target</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>std</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="173" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,8 +617,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +635,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,30 +660,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -635,6 +733,36 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -674,9 +802,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A7FE39D-5614-4A7F-89B7-C167ABC0A251}" name="Movies" displayName="Movies" ref="A1:K42" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:K42" xr:uid="{6A7FE39D-5614-4A7F-89B7-C167ABC0A251}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A7FE39D-5614-4A7F-89B7-C167ABC0A251}" name="Movies" displayName="Movies" ref="A1:Q42" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:Q42" xr:uid="{6A7FE39D-5614-4A7F-89B7-C167ABC0A251}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{5E453F0D-B27C-433C-BF11-BA3FE1A6822E}" name="movie_id"/>
     <tableColumn id="12" xr3:uid="{8D1CEF56-F5B4-4AE0-8193-885474479647}" name="Title"/>
     <tableColumn id="3" xr3:uid="{A73DC6E7-A5B7-4D92-B13E-587CFA363BFA}" name="industry"/>
@@ -684,17 +812,35 @@
     <tableColumn id="5" xr3:uid="{D500D219-E618-40DD-B4AA-E390F996EF1E}" name="imdb_rating"/>
     <tableColumn id="6" xr3:uid="{D06057E5-53B4-474F-BA7C-D7BC731BE502}" name="studio"/>
     <tableColumn id="7" xr3:uid="{70C8CD53-1FFB-4649-B796-093E6560F8C9}" name="language_id"/>
-    <tableColumn id="2" xr3:uid="{89A5598D-B7ED-44E0-8DBE-47762662E0ED}" name="Budget" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{89A5598D-B7ED-44E0-8DBE-47762662E0ED}" name="Budget" dataDxfId="13">
       <calculatedColumnFormula>_xlfn.IFNA(INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Budget]],Financials[#Headers],0)),"Not Avaliable")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{473EABA1-3F76-44E5-A24D-53A4ACA005D1}" name="Revenue" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{473EABA1-3F76-44E5-A24D-53A4ACA005D1}" name="Revenue" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.IFNA(INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Revenue]],Financials[#Headers],0)),"Not Avaliable")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1E8B014C-D5D9-4BF1-929D-71F78B670B6B}" name="Unit" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{1E8B014C-D5D9-4BF1-929D-71F78B670B6B}" name="Unit" dataDxfId="11">
       <calculatedColumnFormula>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Unit]],Financials[#Headers],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E486CEF1-C490-4786-B2CB-B287BB24A8F2}" name="Currency" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{E486CEF1-C490-4786-B2CB-B287BB24A8F2}" name="Currency" dataDxfId="10">
       <calculatedColumnFormula>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{CE44892E-0C5F-41BD-A7BC-C0527C21ACAB}" name="Budget (Mln)" dataDxfId="9">
+      <calculatedColumnFormula>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{EEE5E760-BC1E-443B-B835-FCE0F37DE9DD}" name="Revenue (Mln)" dataDxfId="8">
+      <calculatedColumnFormula>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{6B7E9C02-0D56-4E94-BB14-5B111EE97858}" name="Budget INR" dataDxfId="7">
+      <calculatedColumnFormula>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{1DCF0B2B-9786-419B-A03E-1CFC189A23DC}" name="Revenue INR" dataDxfId="6">
+      <calculatedColumnFormula>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{12F5994C-055D-4404-A746-96CBA3043F7F}" name="Budget USD" dataDxfId="5">
+      <calculatedColumnFormula>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{3C4CAA1F-9BC0-4D6F-A2AF-740949279501}" name="Revenue USD" dataDxfId="4">
+      <calculatedColumnFormula>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -702,7 +848,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}" name="Financials" displayName="Financials" ref="A1:E41" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}" name="Financials" displayName="Financials" ref="A1:E41" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:E41" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D1A9B0F4-FC15-4DC9-80C7-7EBF56996521}" name="movie_id"/>
@@ -716,7 +862,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49E9627B-7F83-4E00-A9BD-B2B85ADBBA2F}" name="actors" displayName="actors" ref="A1:C68" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49E9627B-7F83-4E00-A9BD-B2B85ADBBA2F}" name="actors" displayName="actors" ref="A1:C68" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:C68" xr:uid="{49E9627B-7F83-4E00-A9BD-B2B85ADBBA2F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{17C41506-36D4-4294-9829-5A0C52DE3455}" name="actor_id"/>
@@ -728,7 +874,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69F3DFB9-F7AC-4F5D-9639-8E5EFD749C75}" name="movieactor" displayName="movieactor" ref="A1:B86" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69F3DFB9-F7AC-4F5D-9639-8E5EFD749C75}" name="movieactor" displayName="movieactor" ref="A1:B86" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:B86" xr:uid="{69F3DFB9-F7AC-4F5D-9639-8E5EFD749C75}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{726AA249-607F-4CEE-9C80-419BD67B7D42}" name="movie_id"/>
@@ -739,7 +885,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C058435-0457-4C21-A779-EC166EB5551A}" name="languages" displayName="languages" ref="A1:B9" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C058435-0457-4C21-A779-EC166EB5551A}" name="languages" displayName="languages" ref="A1:B9" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:B9" xr:uid="{1C058435-0457-4C21-A779-EC166EB5551A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E256DBAD-6FC6-4A32-8A1D-C74A5F599F74}" name="language_id"/>
@@ -1012,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView zoomScale="50" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1026,12 +1172,18 @@
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,8 +1217,26 @@
       <c r="K1" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
@@ -1104,8 +1274,32 @@
         <f>_xlfn.IFNA(INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0)),"Not Avaliable")</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>1000</v>
+      </c>
+      <c r="M2">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>12500</v>
+      </c>
+      <c r="N2">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1000</v>
+      </c>
+      <c r="O2">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>12500</v>
+      </c>
+      <c r="P2">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>12.5</v>
+      </c>
+      <c r="Q2">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>156.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -1143,8 +1337,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>200</v>
+      </c>
+      <c r="M3">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>954.8</v>
+      </c>
+      <c r="N3">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>16000</v>
+      </c>
+      <c r="O3">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>76384</v>
+      </c>
+      <c r="P3">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>200</v>
+      </c>
+      <c r="Q3">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>954.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
@@ -1182,8 +1400,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>165</v>
+      </c>
+      <c r="M4">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>644.79999999999995</v>
+      </c>
+      <c r="N4">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>13200</v>
+      </c>
+      <c r="O4">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>51584</v>
+      </c>
+      <c r="P4">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>165</v>
+      </c>
+      <c r="Q4">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>644.79999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -1221,8 +1463,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>180</v>
+      </c>
+      <c r="M5">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>854</v>
+      </c>
+      <c r="N5">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>14400</v>
+      </c>
+      <c r="O5">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>68320</v>
+      </c>
+      <c r="P5">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>180</v>
+      </c>
+      <c r="Q5">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>854</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>105</v>
       </c>
@@ -1260,8 +1526,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>250</v>
+      </c>
+      <c r="M6">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>670</v>
+      </c>
+      <c r="N6">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>20000</v>
+      </c>
+      <c r="O6">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>53600</v>
+      </c>
+      <c r="P6">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>250</v>
+      </c>
+      <c r="Q6">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>106</v>
       </c>
@@ -1299,8 +1589,32 @@
         <f>_xlfn.IFNA(INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0)),"Not Avaliable")</f>
         <v>Not Avaliable</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" t="str">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="N7" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="O7" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="P7" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="Q7" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>107</v>
       </c>
@@ -1338,8 +1652,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>400</v>
+      </c>
+      <c r="M8">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>2000</v>
+      </c>
+      <c r="N8">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>400</v>
+      </c>
+      <c r="O8">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>2000</v>
+      </c>
+      <c r="P8">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108</v>
       </c>
@@ -1377,8 +1715,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>550</v>
+      </c>
+      <c r="M9">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>4000</v>
+      </c>
+      <c r="N9">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>550</v>
+      </c>
+      <c r="O9">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>4000</v>
+      </c>
+      <c r="P9">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>6.875</v>
+      </c>
+      <c r="Q9">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>109</v>
       </c>
@@ -1416,8 +1778,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>390</v>
+      </c>
+      <c r="M10">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>1360</v>
+      </c>
+      <c r="N10">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>390</v>
+      </c>
+      <c r="O10">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>1360</v>
+      </c>
+      <c r="P10">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>4.875</v>
+      </c>
+      <c r="Q10">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>110</v>
       </c>
@@ -1455,8 +1841,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>1400</v>
+      </c>
+      <c r="M11">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>3500</v>
+      </c>
+      <c r="N11">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1400</v>
+      </c>
+      <c r="O11">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>3500</v>
+      </c>
+      <c r="P11">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>17.5</v>
+      </c>
+      <c r="Q11">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>43.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>111</v>
       </c>
@@ -1494,8 +1904,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>25</v>
+      </c>
+      <c r="M12">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>73.3</v>
+      </c>
+      <c r="N12">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>2000</v>
+      </c>
+      <c r="O12">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>5864</v>
+      </c>
+      <c r="P12">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>25</v>
+      </c>
+      <c r="Q12">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>73.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>112</v>
       </c>
@@ -1533,8 +1967,32 @@
         <f>_xlfn.IFNA(INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0)),"Not Avaliable")</f>
         <v>Not Avaliable</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13" t="str">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="M13" t="str">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="N13" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="O13" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="P13" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+      <c r="Q13" t="str">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>Not Avaliable</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>113</v>
       </c>
@@ -1572,8 +2030,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>165</v>
+      </c>
+      <c r="M14">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>701.8</v>
+      </c>
+      <c r="N14">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>13200</v>
+      </c>
+      <c r="O14">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>56144</v>
+      </c>
+      <c r="P14">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>165</v>
+      </c>
+      <c r="Q14">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>701.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>115</v>
       </c>
@@ -1611,8 +2093,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>55</v>
+      </c>
+      <c r="M15">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>307.10000000000002</v>
+      </c>
+      <c r="N15">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>4400</v>
+      </c>
+      <c r="O15">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>24568</v>
+      </c>
+      <c r="P15">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>55</v>
+      </c>
+      <c r="Q15">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>307.10000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>116</v>
       </c>
@@ -1650,8 +2156,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>103</v>
+      </c>
+      <c r="M16">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>460.5</v>
+      </c>
+      <c r="N16">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>8240</v>
+      </c>
+      <c r="O16">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>36840</v>
+      </c>
+      <c r="P16">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>103</v>
+      </c>
+      <c r="Q16">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>460.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>117</v>
       </c>
@@ -1689,8 +2219,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>200</v>
+      </c>
+      <c r="M17">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>2202</v>
+      </c>
+      <c r="N17">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>16000</v>
+      </c>
+      <c r="O17">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>176160</v>
+      </c>
+      <c r="P17">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>200</v>
+      </c>
+      <c r="Q17">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>118</v>
       </c>
@@ -1728,8 +2282,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>3.18</v>
+      </c>
+      <c r="M18">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>3.3</v>
+      </c>
+      <c r="N18">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>254.4</v>
+      </c>
+      <c r="O18">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>264</v>
+      </c>
+      <c r="P18">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>3.18</v>
+      </c>
+      <c r="Q18">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>119</v>
       </c>
@@ -1767,8 +2345,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>237</v>
+      </c>
+      <c r="M19">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>2847</v>
+      </c>
+      <c r="N19">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>18960</v>
+      </c>
+      <c r="O19">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>227760</v>
+      </c>
+      <c r="P19">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>237</v>
+      </c>
+      <c r="Q19">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>120</v>
       </c>
@@ -1806,8 +2408,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>7.2</v>
+      </c>
+      <c r="M20">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>291</v>
+      </c>
+      <c r="N20">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>576</v>
+      </c>
+      <c r="O20">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>23280</v>
+      </c>
+      <c r="P20">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>7.2</v>
+      </c>
+      <c r="Q20">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>121</v>
       </c>
@@ -1845,8 +2471,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>185</v>
+      </c>
+      <c r="M21">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>1006</v>
+      </c>
+      <c r="N21">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>14800</v>
+      </c>
+      <c r="O21">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>80480</v>
+      </c>
+      <c r="P21">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>185</v>
+      </c>
+      <c r="Q21">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>122</v>
       </c>
@@ -1884,8 +2534,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>22</v>
+      </c>
+      <c r="M22">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>322.2</v>
+      </c>
+      <c r="N22">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1760</v>
+      </c>
+      <c r="O22">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>25776</v>
+      </c>
+      <c r="P22">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>22</v>
+      </c>
+      <c r="Q22">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>322.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>123</v>
       </c>
@@ -1923,8 +2597,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>63</v>
+      </c>
+      <c r="M23">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>1046</v>
+      </c>
+      <c r="N23">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>5040</v>
+      </c>
+      <c r="O23">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>83680</v>
+      </c>
+      <c r="P23">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>63</v>
+      </c>
+      <c r="Q23">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>124</v>
       </c>
@@ -1962,8 +2660,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>15.5</v>
+      </c>
+      <c r="M24">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>263.10000000000002</v>
+      </c>
+      <c r="N24">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1240</v>
+      </c>
+      <c r="O24">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>21048</v>
+      </c>
+      <c r="P24">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>15.5</v>
+      </c>
+      <c r="Q24">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>263.10000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>125</v>
       </c>
@@ -2001,8 +2723,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>400</v>
+      </c>
+      <c r="M25">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>2798</v>
+      </c>
+      <c r="N25">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>32000</v>
+      </c>
+      <c r="O25">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>223840</v>
+      </c>
+      <c r="P25">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>400</v>
+      </c>
+      <c r="Q25">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>2798</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>126</v>
       </c>
@@ -2040,8 +2786,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>400</v>
+      </c>
+      <c r="M26">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>2048</v>
+      </c>
+      <c r="N26">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>32000</v>
+      </c>
+      <c r="O26">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>163840</v>
+      </c>
+      <c r="P26">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>400</v>
+      </c>
+      <c r="Q26">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>127</v>
       </c>
@@ -2079,8 +2849,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>70</v>
+      </c>
+      <c r="M27">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>100</v>
+      </c>
+      <c r="N27">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>70</v>
+      </c>
+      <c r="O27">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>100</v>
+      </c>
+      <c r="P27">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>0.875</v>
+      </c>
+      <c r="Q27">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>128</v>
       </c>
@@ -2118,8 +2912,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>120</v>
+      </c>
+      <c r="M28">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>1350</v>
+      </c>
+      <c r="N28">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>120</v>
+      </c>
+      <c r="O28">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>1350</v>
+      </c>
+      <c r="P28">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1.5</v>
+      </c>
+      <c r="Q28">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>16.875</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>129</v>
       </c>
@@ -2157,8 +2975,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>100</v>
+      </c>
+      <c r="M29">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>410</v>
+      </c>
+      <c r="N29">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>100</v>
+      </c>
+      <c r="O29">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>410</v>
+      </c>
+      <c r="P29">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="Q29">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>5.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>124</v>
       </c>
@@ -2196,8 +3038,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>15.5</v>
+      </c>
+      <c r="M30">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>263.10000000000002</v>
+      </c>
+      <c r="N30">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1240</v>
+      </c>
+      <c r="O30">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>21048</v>
+      </c>
+      <c r="P30">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>15.5</v>
+      </c>
+      <c r="Q30">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>263.10000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>105</v>
       </c>
@@ -2235,8 +3101,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>250</v>
+      </c>
+      <c r="M31">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>670</v>
+      </c>
+      <c r="N31">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>20000</v>
+      </c>
+      <c r="O31">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>53600</v>
+      </c>
+      <c r="P31">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>250</v>
+      </c>
+      <c r="Q31">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>130</v>
       </c>
@@ -2274,8 +3164,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>850</v>
+      </c>
+      <c r="M32">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>8540</v>
+      </c>
+      <c r="N32">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>850</v>
+      </c>
+      <c r="O32">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>8540</v>
+      </c>
+      <c r="P32">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>10.625</v>
+      </c>
+      <c r="Q32">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>106.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>131</v>
       </c>
@@ -2313,8 +3227,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>1000</v>
+      </c>
+      <c r="M33">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>5900</v>
+      </c>
+      <c r="N33">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1000</v>
+      </c>
+      <c r="O33">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>5900</v>
+      </c>
+      <c r="P33">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>12.5</v>
+      </c>
+      <c r="Q33">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>73.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>132</v>
       </c>
@@ -2352,8 +3290,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>2000</v>
+      </c>
+      <c r="M34">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>3600</v>
+      </c>
+      <c r="N34">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>2000</v>
+      </c>
+      <c r="O34">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>3600</v>
+      </c>
+      <c r="P34">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>25</v>
+      </c>
+      <c r="Q34">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>133</v>
       </c>
@@ -2391,8 +3353,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>5500</v>
+      </c>
+      <c r="M35">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>12000</v>
+      </c>
+      <c r="N35">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>5500</v>
+      </c>
+      <c r="O35">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>12000</v>
+      </c>
+      <c r="P35">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>68.75</v>
+      </c>
+      <c r="Q35">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>134</v>
       </c>
@@ -2430,8 +3416,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>1800</v>
+      </c>
+      <c r="M36">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>6500</v>
+      </c>
+      <c r="N36">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1800</v>
+      </c>
+      <c r="O36">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>6500</v>
+      </c>
+      <c r="P36">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>22.5</v>
+      </c>
+      <c r="Q36">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>81.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>135</v>
       </c>
@@ -2469,8 +3479,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>250</v>
+      </c>
+      <c r="M37">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>3409</v>
+      </c>
+      <c r="N37">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>250</v>
+      </c>
+      <c r="O37">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>3409</v>
+      </c>
+      <c r="P37">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>3.125</v>
+      </c>
+      <c r="Q37">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>42.612499999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>136</v>
       </c>
@@ -2508,8 +3542,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>900</v>
+      </c>
+      <c r="M38">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>11690</v>
+      </c>
+      <c r="N38">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>900</v>
+      </c>
+      <c r="O38">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>11690</v>
+      </c>
+      <c r="P38">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>11.25</v>
+      </c>
+      <c r="Q38">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>146.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>137</v>
       </c>
@@ -2547,8 +3605,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>216.7</v>
+      </c>
+      <c r="M39">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>370.6</v>
+      </c>
+      <c r="N39">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>17336</v>
+      </c>
+      <c r="O39">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>29648</v>
+      </c>
+      <c r="P39">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>216.7</v>
+      </c>
+      <c r="Q39">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>370.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>138</v>
       </c>
@@ -2586,8 +3668,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>USD</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>177</v>
+      </c>
+      <c r="M40">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>714.4</v>
+      </c>
+      <c r="N40">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>14160</v>
+      </c>
+      <c r="O40">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>57152</v>
+      </c>
+      <c r="P40">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>177</v>
+      </c>
+      <c r="Q40">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>714.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>139</v>
       </c>
@@ -2625,8 +3731,32 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>1800</v>
+      </c>
+      <c r="M41">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>3100</v>
+      </c>
+      <c r="N41">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>1800</v>
+      </c>
+      <c r="O41">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>3100</v>
+      </c>
+      <c r="P41">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>22.5</v>
+      </c>
+      <c r="Q41">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>38.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>140</v>
       </c>
@@ -2664,6 +3794,128 @@
         <f>INDEX(Financials[],MATCH(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[movie_id]:[movie_id]],0),MATCH(Movies[[#Headers],[Currency]],Financials[#Headers],0))</f>
         <v>INR</v>
       </c>
+      <c r="L42">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Budget]]*1000,Movies[[#This Row],[Budget]])</f>
+        <v>500</v>
+      </c>
+      <c r="M42">
+        <f>IF(Movies[[#This Row],[Unit]]="Billions",Movies[[#This Row],[Revenue]]*1000,Movies[[#This Row],[Revenue]])</f>
+        <v>950</v>
+      </c>
+      <c r="N42">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Budget (Mln)]]*80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>500</v>
+      </c>
+      <c r="O42">
+        <f>IF(Movies[[#This Row],[Currency]]="USD",Movies[[#This Row],[Revenue (Mln)]]*80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>950</v>
+      </c>
+      <c r="P42">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Budget (Mln)]]/80,Movies[[#This Row],[Budget (Mln)]])</f>
+        <v>6.25</v>
+      </c>
+      <c r="Q42">
+        <f>IF(Movies[[#This Row],[Currency]]="INR",Movies[[#This Row],[Revenue (Mln)]]/80,Movies[[#This Row],[Revenue (Mln)]])</f>
+        <v>11.875</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N45" t="s">
+        <v>163</v>
+      </c>
+      <c r="O45" t="s">
+        <v>164</v>
+      </c>
+      <c r="P45" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N46" s="3">
+        <f>SUM(Movies[Budget INR])</f>
+        <v>285436.40000000002</v>
+      </c>
+      <c r="O46" s="3">
+        <f>SUM(Movies[Revenue INR])</f>
+        <v>1641789</v>
+      </c>
+      <c r="P46" s="3">
+        <f>SUM(Movies[Budget USD])</f>
+        <v>3567.9549999999999</v>
+      </c>
+      <c r="Q46" s="3">
+        <f>SUM(Movies[Revenue USD])</f>
+        <v>20522.362499999999</v>
+      </c>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>167</v>
+      </c>
+      <c r="H49">
+        <f>COUNTA(Movies[movie_id])</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>168</v>
+      </c>
+      <c r="H50">
+        <f>COUNTIF(Movies[industry],"Bollywood")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51">
+        <f>COUNTIF(Movies[industry],"Hollywood")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>169</v>
+      </c>
+      <c r="H52">
+        <f>SUMIF(Movies[industry],"Bollywood",Movies[Budget INR])</f>
+        <v>18630</v>
+      </c>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G53" t="s">
+        <v>170</v>
+      </c>
+      <c r="H53">
+        <f>SUMIF(Movies[industry],"bollywood",Movies[Revenue INR])</f>
+        <v>80909</v>
+      </c>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>171</v>
+      </c>
+      <c r="H54">
+        <f>AVERAGE(H53,H50)</f>
+        <v>40463.5</v>
+      </c>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>172</v>
+      </c>
+      <c r="H55" s="4">
+        <f>H53/O46</f>
+        <v>4.9280997740879004E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="H56" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2676,6 +3928,161 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F2B53F-D7C5-4CB3-9B21-6FB537FFE058}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="8">
+        <f>SUMIF(Movies[studio],"Marvel Studios",Movies[Revenue USD])</f>
+        <v>9724.6</v>
+      </c>
+      <c r="C2" s="8">
+        <v>8000</v>
+      </c>
+      <c r="D2" s="8">
+        <f>B2-C2</f>
+        <v>1724.6000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="8">
+        <f>SUMIF(Movies[studio],"Marvel Studios",Movies[Budget USD])</f>
+        <v>2238.6999999999998</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2000</v>
+      </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D4" si="0">B3-C3</f>
+        <v>238.69999999999982</v>
+      </c>
+      <c r="G3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(Movies[imdb_rating])</f>
+        <v>7.9325000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="8">
+        <f>B2-B3</f>
+        <v>7485.9000000000005</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6000</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>1485.9000000000005</v>
+      </c>
+      <c r="G4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H4">
+        <f>MEDIAN(Movies[imdb_rating])</f>
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="7">
+        <f>B4/B3</f>
+        <v>3.3438602760530669</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9">
+        <f>B5/C5</f>
+        <v>1.114620092017689</v>
+      </c>
+      <c r="G5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H5">
+        <f>MODE(Movies[imdb_rating])</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="6">
+        <f>B2/SUMIF(Movies[industry],"Hollywood",Movies[Revenue USD])</f>
+        <v>0.49841627799702731</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D6" s="10">
+        <f>B6-C6</f>
+        <v>-5.1583722002972732E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="12">
+        <f>_xlfn.VAR.P(Movies[imdb_rating])</f>
+        <v>1.3301937500000076</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="G7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H7" s="11">
+        <f>_xlfn.STDEV.P(Movies[imdb_rating])</f>
+        <v>1.1533402576863463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF951C0-D968-407B-BACE-9EC26BF67B79}">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -3394,7 +4801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6805207-AD4A-4BA5-928C-E78006753CCF}">
   <dimension ref="A1:C68"/>
   <sheetViews>
@@ -4164,7 +5571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B42F180-645C-4BD4-BB22-B680DB6CAFAD}">
   <dimension ref="A1:B86"/>
   <sheetViews>
@@ -4873,7 +6280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F2F15D-C7E5-45CD-9337-3706D6E911A4}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -4967,6 +6374,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MediaLengthInSeconds xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824" xsi:nil="true"/>
+    <SharedWithUsers xmlns="46297aa2-77d1-4586-9726-07d56a535ee7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100686C0266E115364AA9B96DE5BECF7DB6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c921848065db5a49d1de2391ec81580e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="631564f6-0349-4cc5-b00d-7cf3ba42f824" xmlns:ns3="46297aa2-77d1-4586-9726-07d56a535ee7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff9dd1b7eff9d7fccc1b7fb333026bb0" ns2:_="" ns3:_="">
     <xsd:import namespace="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
@@ -5195,35 +6630,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MediaLengthInSeconds xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824" xsi:nil="true"/>
-    <SharedWithUsers xmlns="46297aa2-77d1-4586-9726-07d56a535ee7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEFF9027-FBEF-4910-8EE6-13D64012C7E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
+    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C97D6F-A515-40FC-959A-7BC863F10CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02BA008F-2FD2-4901-8027-A024DA31C6C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5240,23 +6666,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEFF9027-FBEF-4910-8EE6-13D64012C7E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
-    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C97D6F-A515-40FC-959A-7BC863F10CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>